<commit_message>
change the font size
</commit_message>
<xml_diff>
--- a/m2.xlsx
+++ b/m2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\GIT\manivarsha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEB359-EE51-4253-B9AD-D7701EBB4DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71978FA8-AA7C-452F-BB18-418B1B4D270C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -102,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +99,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -127,12 +142,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +521,7 @@
   <dimension ref="D3:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,448 +529,506 @@
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="4:15" ht="22.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D4">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>35</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>52</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>35</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>40</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>20</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <f>L4/5</f>
         <v>36.4</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <f>SUM(F4:J4)</f>
         <v>182</v>
       </c>
-      <c r="N4">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3">
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <f>VLOOKUP(N4,D3:L15,9,0)</f>
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D5">
+    <row r="5" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>50</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>53</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>37</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="6">
         <v>43</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <v>24</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="6">
         <f t="shared" ref="K5:K15" si="0">L5/5</f>
         <v>41.4</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="6">
         <f t="shared" ref="L5:L15" si="1">SUM(F5:J5)</f>
         <v>207</v>
       </c>
-      <c r="N5">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D6">
+      <c r="O5" s="7">
+        <f t="shared" ref="O5:O15" si="2">VLOOKUP(N5,D4:L16,9,0)</f>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>54</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>54</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>39</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="6">
         <v>46</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="6">
         <v>28</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="6">
         <f t="shared" si="0"/>
         <v>44.2</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="6">
         <f t="shared" si="1"/>
         <v>221</v>
       </c>
-      <c r="N6">
+      <c r="M6" s="6"/>
+      <c r="N6" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D7">
+      <c r="O6" s="7">
+        <f t="shared" si="2"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>56</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>55</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>41</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="6">
         <v>49</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <v>32</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="6">
         <f t="shared" si="0"/>
         <v>46.6</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="6">
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
-      <c r="N7">
+      <c r="M7" s="6"/>
+      <c r="N7" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8">
+      <c r="O7" s="7">
+        <f t="shared" si="2"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>45</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>56</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>43</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="6">
         <v>52</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <v>36</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="6">
         <f t="shared" si="0"/>
         <v>46.4</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="6">
         <f t="shared" si="1"/>
         <v>232</v>
       </c>
-      <c r="N8">
+      <c r="M8" s="6"/>
+      <c r="N8" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D9">
+      <c r="O8" s="7">
+        <f t="shared" si="2"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D9" s="5">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>56</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>57</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>45</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="6">
         <v>55</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <v>40</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="6">
         <f t="shared" si="0"/>
         <v>50.6</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="6">
         <f t="shared" si="1"/>
         <v>253</v>
       </c>
-      <c r="N9">
+      <c r="M9" s="6"/>
+      <c r="N9" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D10">
+      <c r="O9" s="7">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D10" s="5">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>46</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>58</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>47</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="6">
         <v>58</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="6">
         <v>44</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="6">
         <f t="shared" si="0"/>
         <v>50.6</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <f t="shared" si="1"/>
         <v>253</v>
       </c>
-      <c r="N10">
+      <c r="M10" s="6"/>
+      <c r="N10" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D11">
+      <c r="O10" s="7">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D11" s="5">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>41</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>59</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="6">
         <v>49</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="6">
         <v>61</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="6">
         <v>48</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="6">
         <f t="shared" si="0"/>
         <v>51.6</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="6">
         <f t="shared" si="1"/>
         <v>258</v>
       </c>
-      <c r="N11">
+      <c r="M11" s="6"/>
+      <c r="N11" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D12">
+      <c r="O11" s="7">
+        <f t="shared" si="2"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D12" s="5">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>75</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>60</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>51</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <v>64</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <v>52</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="6">
         <f t="shared" si="0"/>
         <v>60.4</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="6">
         <f t="shared" si="1"/>
         <v>302</v>
       </c>
-      <c r="N12">
+      <c r="M12" s="6"/>
+      <c r="N12" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D13">
+      <c r="O12" s="7">
+        <f t="shared" si="2"/>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>65</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <v>61</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="6">
         <v>53</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="6">
         <v>67</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="6">
         <v>56</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="6">
         <f t="shared" si="0"/>
         <v>60.4</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="6">
         <f t="shared" si="1"/>
         <v>302</v>
       </c>
-      <c r="N13">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D14">
+      <c r="O13" s="7">
+        <f t="shared" si="2"/>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D14" s="5">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>54</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <v>62</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>55</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="6">
         <v>70</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="6">
         <v>60</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="6">
         <f t="shared" si="0"/>
         <v>60.2</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <f t="shared" si="1"/>
         <v>301</v>
       </c>
-      <c r="N14">
+      <c r="M14" s="6"/>
+      <c r="N14" s="6">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D15">
+      <c r="O14" s="7">
+        <f t="shared" si="2"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="4:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="8">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="9">
         <v>52</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>63</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="9">
         <v>57</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="9">
         <v>73</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="9">
         <v>64</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="9">
         <f t="shared" si="0"/>
         <v>61.8</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="9">
         <f t="shared" si="1"/>
         <v>309</v>
       </c>
-      <c r="N15">
+      <c r="M15" s="9"/>
+      <c r="N15" s="9">
         <v>12</v>
+      </c>
+      <c r="O15" s="10">
+        <f t="shared" si="2"/>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>